<commit_message>
got rid of food as an expense since I plan on breaking even
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c2c6e3652e668e7/Work/Projects/dogen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD868E3D-F417-4930-9F78-D05A92124599}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8AD896DE-910B-4434-A062-D30D3C1149A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Overhead</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Uncontrollable Profit Variables</t>
+  </si>
+  <si>
+    <t>charge by rounding up to the nearest dollar</t>
+  </si>
+  <si>
+    <t>security, food, greeting desk</t>
+  </si>
+  <si>
+    <t>I will be maintenance</t>
   </si>
 </sst>
 </file>
@@ -496,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E200A4BF-7444-461A-A7D9-DCB85EAD9C4B}">
-  <dimension ref="A2:B38"/>
+  <dimension ref="A2:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,31 +517,37 @@
     <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>700</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -541,7 +556,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -550,7 +565,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -559,7 +574,7 @@
         <v>107100</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -567,15 +582,18 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -583,7 +601,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -591,7 +609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -599,22 +617,22 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1">
         <f>SUM(B8:B12)</f>
-        <v>6700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1">
         <f>B13*12+B7</f>
-        <v>187500</v>
+        <v>175500</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +775,7 @@
       </c>
       <c r="B38" s="1">
         <f>B37-B14</f>
-        <v>53475</v>
+        <v>65475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>